<commit_message>
update Fig3 and Fig4
Different DI and OI trials 5,10 and 15 data; Redo Fig3 figure
</commit_message>
<xml_diff>
--- a/Bayes_Estimation_paper/need to check/Fig3_trials_5.xlsx
+++ b/Bayes_Estimation_paper/need to check/Fig3_trials_5.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7320865-1CF2-4F79-A587-8A02BED5275E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="490" yWindow="3260" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="490" yWindow="3260" windowWidth="19200" windowHeight="11170"/>
   </bookViews>
   <sheets>
     <sheet name="rp" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="angle" sheetId="6" r:id="rId4"/>
     <sheet name="sigma" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -45,7 +45,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,12 +53,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -375,63 +377,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="2.1796875" customWidth="1"/>
-    <col min="2" max="5" width="4.7265625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="true"/>
+    <col min="2" max="2" width="4.7109375" customWidth="true"/>
+    <col min="3" max="3" width="4.7109375" customWidth="true"/>
+    <col min="4" max="4" width="4.7109375" customWidth="true"/>
+    <col min="5" max="5" width="4.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0.2</v>
-      </c>
-      <c r="C1">
-        <v>0.32</v>
-      </c>
-      <c r="D1">
-        <v>0.3</v>
-      </c>
-      <c r="E1">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.85</v>
-      </c>
-      <c r="C2">
-        <v>0.59</v>
-      </c>
-      <c r="D2">
-        <v>0.59</v>
-      </c>
-      <c r="E2">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0.95</v>
-      </c>
-      <c r="C3">
-        <v>0.93</v>
-      </c>
-      <c r="D3">
-        <v>0.91</v>
-      </c>
-      <c r="E3">
-        <v>0.74</v>
+    <row r="1">
+      <c r="A1" s="0">
+        <v>0.089999999999999997</v>
+      </c>
+      <c r="B1" s="0">
+        <v>0.17000000000000001</v>
+      </c>
+      <c r="C1" s="0">
+        <v>0.29999999999999999</v>
+      </c>
+      <c r="D1" s="0">
+        <v>0.29999999999999999</v>
+      </c>
+      <c r="E1" s="0">
+        <v>0.17999999999999999</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>0.35999999999999999</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.82999999999999996</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.58999999999999997</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.58999999999999997</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.42999999999999999</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>0.75</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0.94999999999999996</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.93000000000000005</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.92000000000000004</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0.71999999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -448,58 +453,62 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="5" width="4.7265625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="true"/>
+    <col min="2" max="2" width="4.7109375" customWidth="true"/>
+    <col min="3" max="3" width="4.7109375" customWidth="true"/>
+    <col min="4" max="4" width="4.7109375" customWidth="true"/>
+    <col min="5" max="5" width="4.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1">
+    <row r="1">
+      <c r="A1" s="0">
         <v>0.22</v>
       </c>
-      <c r="B1">
-        <v>0.11</v>
-      </c>
-      <c r="C1">
-        <v>0.13</v>
-      </c>
-      <c r="D1">
-        <v>0.18</v>
-      </c>
-      <c r="E1">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+      <c r="B1" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="C1" s="0">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="D1" s="0">
+        <v>0.17000000000000001</v>
+      </c>
+      <c r="E1" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
         <v>0.28000000000000003</v>
       </c>
-      <c r="B2">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="C2">
-        <v>0.31</v>
-      </c>
-      <c r="D2">
-        <v>0.34</v>
-      </c>
-      <c r="E2">
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>0.3</v>
-      </c>
-      <c r="B3">
-        <v>0.94</v>
-      </c>
-      <c r="C3">
-        <v>0.82</v>
-      </c>
-      <c r="D3">
-        <v>0.63</v>
-      </c>
-      <c r="E3">
-        <v>0.71</v>
+      <c r="B2" s="0">
+        <v>0.29999999999999999</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.32000000000000001</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.34999999999999998</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.46000000000000002</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>0.29999999999999999</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0.93999999999999995</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.81999999999999995</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.62</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0.68999999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -516,57 +525,61 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="5" width="4.7265625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="true"/>
+    <col min="2" max="2" width="4.7109375" customWidth="true"/>
+    <col min="3" max="3" width="4.7109375" customWidth="true"/>
+    <col min="4" max="4" width="4.7109375" customWidth="true"/>
+    <col min="5" max="5" width="4.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1">
-        <v>0.51</v>
-      </c>
-      <c r="B1">
+    <row r="1">
+      <c r="A1" s="0">
+        <v>0.51000000000000001</v>
+      </c>
+      <c r="B1" s="0">
         <v>0.28999999999999998</v>
       </c>
-      <c r="C1">
-        <v>0.34</v>
-      </c>
-      <c r="D1">
+      <c r="C1" s="0">
+        <v>0.34000000000000002</v>
+      </c>
+      <c r="D1" s="0">
         <v>0.31</v>
       </c>
-      <c r="E1">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>0.54</v>
-      </c>
-      <c r="B2">
+      <c r="E1" s="0">
+        <v>0.95999999999999996</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B2" s="0">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C2">
-        <v>0.68</v>
-      </c>
-      <c r="D2">
-        <v>0.68</v>
-      </c>
-      <c r="E2">
+      <c r="C2" s="0">
+        <v>0.68000000000000005</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.68000000000000005</v>
+      </c>
+      <c r="E2" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>0.74</v>
-      </c>
-      <c r="B3">
-        <v>0.85</v>
-      </c>
-      <c r="C3">
+    <row r="3">
+      <c r="A3" s="0">
+        <v>0.73999999999999999</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0.84999999999999998</v>
+      </c>
+      <c r="C3" s="0">
         <v>0.88</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>0.88</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>1</v>
       </c>
     </row>
@@ -584,58 +597,62 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="5" width="4.7265625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="true"/>
+    <col min="2" max="2" width="4.7109375" customWidth="true"/>
+    <col min="3" max="3" width="4.7109375" customWidth="true"/>
+    <col min="4" max="4" width="4.7109375" customWidth="true"/>
+    <col min="5" max="5" width="4.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1">
-        <v>0.03</v>
-      </c>
-      <c r="B1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C1">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="D1">
-        <v>0.32</v>
-      </c>
-      <c r="E1">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+    <row r="1">
+      <c r="A1" s="0">
+        <v>0.029999999999999999</v>
+      </c>
+      <c r="B1" s="0">
+        <v>0.059999999999999998</v>
+      </c>
+      <c r="C1" s="0">
+        <v>0.23000000000000001</v>
+      </c>
+      <c r="D1" s="0">
         <v>0.31</v>
       </c>
-      <c r="B2">
-        <v>0.65</v>
-      </c>
-      <c r="C2">
-        <v>0.68</v>
-      </c>
-      <c r="D2">
+      <c r="E1" s="0">
+        <v>0.77000000000000002</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>0.31</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.66000000000000003</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.68000000000000005</v>
+      </c>
+      <c r="D2" s="0">
         <v>0.5</v>
       </c>
-      <c r="E2">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>0.46</v>
-      </c>
-      <c r="B3">
-        <v>0.8</v>
-      </c>
-      <c r="C3">
-        <v>0.85</v>
-      </c>
-      <c r="D3">
-        <v>0.85</v>
-      </c>
-      <c r="E3">
-        <v>0.83</v>
+      <c r="E2" s="0">
+        <v>0.77000000000000002</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>0.46000000000000002</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.84999999999999998</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.84999999999999998</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0.82999999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -652,58 +669,62 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="5" width="4.7265625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="true"/>
+    <col min="2" max="2" width="4.7109375" customWidth="true"/>
+    <col min="3" max="3" width="4.7109375" customWidth="true"/>
+    <col min="4" max="4" width="4.7109375" customWidth="true"/>
+    <col min="5" max="5" width="4.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1">
+    <row r="1">
+      <c r="A1" s="0">
         <v>0.01</v>
       </c>
-      <c r="B1">
-        <v>0.03</v>
-      </c>
-      <c r="C1">
-        <v>0.09</v>
-      </c>
-      <c r="D1">
-        <v>0.3</v>
-      </c>
-      <c r="E1">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>0.08</v>
-      </c>
-      <c r="B2">
-        <v>0.06</v>
-      </c>
-      <c r="C2">
-        <v>0.17</v>
-      </c>
-      <c r="D2">
-        <v>0.47</v>
-      </c>
-      <c r="E2">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>0.91</v>
-      </c>
-      <c r="B3">
-        <v>0.92</v>
-      </c>
-      <c r="C3">
-        <v>0.84</v>
-      </c>
-      <c r="D3">
-        <v>0.73</v>
-      </c>
-      <c r="E3">
-        <v>0.88</v>
+      <c r="B1" s="0">
+        <v>0.029999999999999999</v>
+      </c>
+      <c r="C1" s="0">
+        <v>0.080000000000000002</v>
+      </c>
+      <c r="D1" s="0">
+        <v>0.33000000000000002</v>
+      </c>
+      <c r="E1" s="0">
+        <v>0.34999999999999998</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>0.080000000000000002</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.059999999999999998</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.17000000000000001</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.47999999999999998</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.64000000000000001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>0.91000000000000003</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0.92000000000000004</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.83999999999999997</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.72999999999999998</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0.90000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>